<commit_message>
LuLa: updated to mitigate risk: KaJa, PiSm
</commit_message>
<xml_diff>
--- a/agenda/agenda_07_02.xlsx
+++ b/agenda/agenda_07_02.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="62">
   <si>
     <t>Rano</t>
   </si>
@@ -62,53 +62,166 @@
     <t>12+ (4 os.)</t>
   </si>
   <si>
-    <t>8+ (6 os.)</t>
-  </si>
-  <si>
-    <t>Kasia, 
-Piotrek S.</t>
-  </si>
-  <si>
-    <t>Tomek,
-Piotrek K.</t>
-  </si>
-  <si>
-    <t>Piotrek K.
-Jacek</t>
-  </si>
-  <si>
     <t>Tomek,
 Dawid.</t>
   </si>
   <si>
+    <t>6+ (4 os.)</t>
+  </si>
+  <si>
+    <t>Piotr S.</t>
+  </si>
+  <si>
+    <t>8+ (4 os.)</t>
+  </si>
+  <si>
+    <t>10+ (4 os.)</t>
+  </si>
+  <si>
     <t>Krzysiu, 
-Kasia</t>
-  </si>
-  <si>
-    <t>Krzysiu, 
-Lukasz G.,
+Zuza</t>
+  </si>
+  <si>
+    <t>Lukasz G.
+Jacek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tomek,
+Lukasz G. </t>
+  </si>
+  <si>
+    <t>Piotrek S. ??
+Piorek K.
 Marcin</t>
   </si>
   <si>
-    <t>6+ (4 os.)</t>
-  </si>
-  <si>
-    <t>10+ (6 os.)</t>
-  </si>
-  <si>
-    <t>Piotr S.</t>
-  </si>
-  <si>
-    <t>Lukasz G.,
+    <t>Lukasz L.</t>
+  </si>
+  <si>
+    <t>Piotr S. ??/ Lukasz L.</t>
+  </si>
+  <si>
+    <t>Piotrek K,
 Dawid,
-Lukasz L.</t>
+Lukasz L. ??</t>
+  </si>
+  <si>
+    <t>Marcin M.</t>
+  </si>
+  <si>
+    <t>sphero:</t>
+  </si>
+  <si>
+    <t>Piotrek K</t>
+  </si>
+  <si>
+    <t>robogames:</t>
+  </si>
+  <si>
+    <t>zakupy catering:</t>
+  </si>
+  <si>
+    <t>zakupy pod lutowanie:</t>
+  </si>
+  <si>
+    <t>Tomek</t>
+  </si>
+  <si>
+    <t>gadżety/upominki</t>
+  </si>
+  <si>
+    <t>Piotrek S./Zuza</t>
+  </si>
+  <si>
+    <t>wszyscy</t>
+  </si>
+  <si>
+    <t>kompy:</t>
+  </si>
+  <si>
+    <t>przygotowanie sal (piątek):</t>
+  </si>
+  <si>
+    <t>soft:</t>
+  </si>
+  <si>
+    <t>iPady:</t>
+  </si>
+  <si>
+    <t>community (1 szt.), Piotrek K</t>
+  </si>
+  <si>
+    <t>tablety:</t>
+  </si>
+  <si>
+    <t>community (1 szt.) + Lukasz L.</t>
+  </si>
+  <si>
+    <t>LEGO:</t>
+  </si>
+  <si>
+    <t>Dawid + LuLa (demo)</t>
+  </si>
+  <si>
+    <t>arduino:</t>
+  </si>
+  <si>
+    <t>Jacek</t>
+  </si>
+  <si>
+    <t>zadnia na pendrive'y:</t>
+  </si>
+  <si>
+    <t>Krzysiu</t>
+  </si>
+  <si>
+    <t>etykietki:</t>
+  </si>
+  <si>
+    <t>dyplomy:</t>
+  </si>
+  <si>
+    <t>baterie / ladowarka</t>
+  </si>
+  <si>
+    <t>sale bookowanie (PLUMy -&gt; Piotr S.)/rzutniki/podzial sal</t>
+  </si>
+  <si>
+    <t>PLUM 1+2, PLUM3 (zglosic Dorocie)</t>
+  </si>
+  <si>
+    <t>zgloszenie event'u</t>
+  </si>
+  <si>
+    <t>Ochrona/Magda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pizza: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Koordynator </t>
+  </si>
+  <si>
+    <t xml:space="preserve">proste menu </t>
+  </si>
+  <si>
+    <t>+ picie do obiadu osobno</t>
+  </si>
+  <si>
+    <t>Uwagi</t>
+  </si>
+  <si>
+    <t>Kto</t>
+  </si>
+  <si>
+    <t>Co</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,8 +251,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -168,6 +288,11 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -178,14 +303,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
@@ -196,12 +322,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="5"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
     <cellStyle name="60% - Accent1" xfId="4" builtinId="32"/>
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="5" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -497,7 +626,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -511,20 +640,21 @@
     <col min="8" max="8" width="17.5703125" customWidth="1"/>
     <col min="9" max="9" width="16.140625" customWidth="1"/>
     <col min="11" max="11" width="13.42578125" customWidth="1"/>
+    <col min="12" max="12" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1" t="s">
@@ -535,7 +665,7 @@
         <v>6</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="64.5" customHeight="1">
@@ -546,25 +676,25 @@
         <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="96.75" customHeight="1">
@@ -575,7 +705,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>7</v>
@@ -587,7 +717,7 @@
         <v>4</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>5</v>
@@ -604,12 +734,195 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="55.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>

<commit_message>
LuLa: update after meeting
</commit_message>
<xml_diff>
--- a/agenda/agenda_07_02.xlsx
+++ b/agenda/agenda_07_02.xlsx
@@ -7,16 +7,15 @@
     <workbookView xWindow="360" yWindow="60" windowWidth="11295" windowHeight="5580" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
-    <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
-    <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
+    <sheet name="Agenda_Sale" sheetId="1" r:id="rId1"/>
+    <sheet name="ActionPlan" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="89">
   <si>
     <t>Rano</t>
   </si>
@@ -55,205 +54,262 @@
 (+ zabezpieczenie LeOS)</t>
   </si>
   <si>
+    <t>12+ (4 os.)</t>
+  </si>
+  <si>
+    <t>6+ (4 os.)</t>
+  </si>
+  <si>
+    <t>Piotr S.</t>
+  </si>
+  <si>
+    <t>8+ (4 os.)</t>
+  </si>
+  <si>
+    <t>10+ (4 os.)</t>
+  </si>
+  <si>
+    <t>Lukasz L.</t>
+  </si>
+  <si>
+    <t>Marcin M.</t>
+  </si>
+  <si>
+    <t>sphero:</t>
+  </si>
+  <si>
+    <t>Piotrek K</t>
+  </si>
+  <si>
+    <t>robogames:</t>
+  </si>
+  <si>
+    <t>zakupy catering:</t>
+  </si>
+  <si>
+    <t>zakupy pod lutowanie:</t>
+  </si>
+  <si>
+    <t>Tomek</t>
+  </si>
+  <si>
+    <t>gadżety/upominki</t>
+  </si>
+  <si>
+    <t>Piotrek S./Zuza</t>
+  </si>
+  <si>
+    <t>wszyscy</t>
+  </si>
+  <si>
+    <t>kompy:</t>
+  </si>
+  <si>
+    <t>przygotowanie sal (piątek):</t>
+  </si>
+  <si>
+    <t>soft:</t>
+  </si>
+  <si>
+    <t>iPady:</t>
+  </si>
+  <si>
+    <t>community (1 szt.), Piotrek K</t>
+  </si>
+  <si>
+    <t>tablety:</t>
+  </si>
+  <si>
+    <t>community (1 szt.) + Lukasz L.</t>
+  </si>
+  <si>
+    <t>LEGO:</t>
+  </si>
+  <si>
+    <t>Dawid + LuLa (demo)</t>
+  </si>
+  <si>
+    <t>arduino:</t>
+  </si>
+  <si>
+    <t>Jacek</t>
+  </si>
+  <si>
+    <t>zadnia na pendrive'y:</t>
+  </si>
+  <si>
+    <t>Krzysiu</t>
+  </si>
+  <si>
+    <t>etykietki:</t>
+  </si>
+  <si>
+    <t>dyplomy:</t>
+  </si>
+  <si>
+    <t>sale bookowanie (PLUMy -&gt; Piotr S.)/rzutniki/podzial sal</t>
+  </si>
+  <si>
+    <t>Ochrona/Magda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pizza: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Koordynator </t>
+  </si>
+  <si>
+    <t>Uwagi</t>
+  </si>
+  <si>
+    <t>Kto</t>
+  </si>
+  <si>
+    <t>Co</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>dodatkowe załatwione (będą 2)</t>
+  </si>
+  <si>
+    <t>+ picie do obiadu osobno, zamowic dzien wczesniej (na 12:30)</t>
+  </si>
+  <si>
+    <t>jeszcze nie ta edycja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piotr S. pisze do comm. </t>
+  </si>
+  <si>
+    <t>kupione! MaMo pomoże przy foliach</t>
+  </si>
+  <si>
+    <t>Lukasz L: w repo folder (wrzucić zadania do środy 4II)</t>
+  </si>
+  <si>
+    <t>budżet na koszulki? Pendrive'y sa (4 II). Notatniki ok., torebki (?)</t>
+  </si>
+  <si>
+    <t>dzień wcześniej!! ;-)</t>
+  </si>
+  <si>
+    <t>PLUM 1+2, PLUM3 (zglosic Dorocie &lt; Piotr S.)</t>
+  </si>
+  <si>
+    <t>baterie sa, ladowarka - ciezko (zakup raczej)</t>
+  </si>
+  <si>
+    <t>baterie / ladowarka:</t>
+  </si>
+  <si>
+    <t>zgloszenie event'u:</t>
+  </si>
+  <si>
+    <t>proste menu, dzień wcześniej!! ;-)</t>
+  </si>
+  <si>
+    <t>przygotowanie demo:</t>
+  </si>
+  <si>
+    <t>zebrać materiał:</t>
+  </si>
+  <si>
+    <t>zdjęcia, montaż, klip</t>
+  </si>
+  <si>
+    <t>4: Zuza, Tomek L, Lukasz L, Dawid?</t>
+  </si>
+  <si>
+    <t>Piotr S./Lukasz L.</t>
+  </si>
+  <si>
+    <t>ok.</t>
+  </si>
+  <si>
+    <t>będzie</t>
+  </si>
+  <si>
+    <t>będzie, krata: 50x50</t>
+  </si>
+  <si>
+    <t>pendrive na razie stare - sa
+zeszyty sa
+olowki przyjda 
+koszulki się drukuja - będą!!!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sobota rano: 8:30, oznaczyc monitory (nalepka z wlascicielem), </t>
+  </si>
+  <si>
+    <t>Tomek,
+Dawid.
+Lukasz L. - sport
+[PLUM 1 + PLUM2]</t>
+  </si>
+  <si>
+    <t>Tomek,
+Lukasz G. 
+[PLUM 1 + PLUM2]</t>
+  </si>
+  <si>
+    <t>Piotrek S.
+Piorek K.
+Marcin
+[PLUM 3]</t>
+  </si>
+  <si>
     <t>Jacek, 
-Marcin</t>
-  </si>
-  <si>
-    <t>12+ (4 os.)</t>
-  </si>
-  <si>
-    <t>Tomek,
-Dawid.</t>
-  </si>
-  <si>
-    <t>6+ (4 os.)</t>
-  </si>
-  <si>
-    <t>Piotr S.</t>
-  </si>
-  <si>
-    <t>8+ (4 os.)</t>
-  </si>
-  <si>
-    <t>10+ (4 os.)</t>
-  </si>
-  <si>
-    <t>Krzysiu, 
-Zuza</t>
+Marcin
+[PLUM3]</t>
   </si>
   <si>
     <t>Lukasz G.
-Jacek</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tomek,
-Lukasz G. </t>
-  </si>
-  <si>
-    <t>Piotrek S. ??
-Piorek K.
-Marcin</t>
-  </si>
-  <si>
-    <t>Lukasz L.</t>
-  </si>
-  <si>
-    <t>Piotr S. ??/ Lukasz L.</t>
+Jacek
+[5 przy CHILLOUT]</t>
   </si>
   <si>
     <t>Piotrek K,
 Dawid,
-Lukasz L. ??</t>
-  </si>
-  <si>
-    <t>Marcin M.</t>
-  </si>
-  <si>
-    <t>sphero:</t>
-  </si>
-  <si>
-    <t>Piotrek K</t>
-  </si>
-  <si>
-    <t>robogames:</t>
-  </si>
-  <si>
-    <t>zakupy catering:</t>
-  </si>
-  <si>
-    <t>zakupy pod lutowanie:</t>
-  </si>
-  <si>
-    <t>Tomek</t>
-  </si>
-  <si>
-    <t>gadżety/upominki</t>
-  </si>
-  <si>
-    <t>Piotrek S./Zuza</t>
-  </si>
-  <si>
-    <t>wszyscy</t>
-  </si>
-  <si>
-    <t>kompy:</t>
-  </si>
-  <si>
-    <t>przygotowanie sal (piątek):</t>
-  </si>
-  <si>
-    <t>soft:</t>
-  </si>
-  <si>
-    <t>iPady:</t>
-  </si>
-  <si>
-    <t>community (1 szt.), Piotrek K</t>
-  </si>
-  <si>
-    <t>tablety:</t>
-  </si>
-  <si>
-    <t>community (1 szt.) + Lukasz L.</t>
-  </si>
-  <si>
-    <t>LEGO:</t>
-  </si>
-  <si>
-    <t>Dawid + LuLa (demo)</t>
-  </si>
-  <si>
-    <t>arduino:</t>
-  </si>
-  <si>
-    <t>Jacek</t>
-  </si>
-  <si>
-    <t>zadnia na pendrive'y:</t>
-  </si>
-  <si>
-    <t>Krzysiu</t>
-  </si>
-  <si>
-    <t>etykietki:</t>
-  </si>
-  <si>
-    <t>dyplomy:</t>
-  </si>
-  <si>
-    <t>sale bookowanie (PLUMy -&gt; Piotr S.)/rzutniki/podzial sal</t>
-  </si>
-  <si>
-    <t>Ochrona/Magda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pizza: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Koordynator </t>
-  </si>
-  <si>
-    <t>Uwagi</t>
-  </si>
-  <si>
-    <t>Kto</t>
-  </si>
-  <si>
-    <t>Co</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>dodatkowe załatwione (będą 2)</t>
-  </si>
-  <si>
-    <t>+ picie do obiadu osobno, zamowic dzien wczesniej (na 12:30)</t>
-  </si>
-  <si>
-    <t>jeszcze nie ta edycja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Piotr S. pisze do comm. </t>
-  </si>
-  <si>
-    <t>kupione! MaMo pomoże przy foliach</t>
-  </si>
-  <si>
-    <t>Lukasz L: w repo folder (wrzucić zadania do środy 4II)</t>
-  </si>
-  <si>
-    <t>budżet na koszulki? Pendrive'y sa (4 II). Notatniki ok., torebki (?)</t>
-  </si>
-  <si>
-    <t>dzień wcześniej!! ;-)</t>
-  </si>
-  <si>
-    <t>PLUM 1+2, PLUM3 (zglosic Dorocie &lt; Piotr S.)</t>
-  </si>
-  <si>
-    <t>baterie sa, ladowarka - ciezko (zakup raczej)</t>
-  </si>
-  <si>
-    <t>baterie / ladowarka:</t>
-  </si>
-  <si>
-    <t>zgloszenie event'u:</t>
-  </si>
-  <si>
-    <t>proste menu, dzień wcześniej!! ;-)</t>
-  </si>
-  <si>
-    <t>przygotowanie demo:</t>
-  </si>
-  <si>
-    <t>zebrać materiał:</t>
-  </si>
-  <si>
-    <t>zdjęcia, montaż, klip</t>
-  </si>
-  <si>
-    <t>4: Zuza, Tomek L, Lukasz L, Dawid?</t>
+Lukasz L.
+[5 przy CHILLOUT]</t>
+  </si>
+  <si>
+    <t>Krzysiu, 
+Zuza (sport)
+[7.10]</t>
+  </si>
+  <si>
+    <t>Krzysiu, 
+Zuza
+[7.10]</t>
+  </si>
+  <si>
+    <t>wgrac soft!!!</t>
+  </si>
+  <si>
+    <t>Lukasz L + Piotr K.</t>
+  </si>
+  <si>
+    <t>zlozyc lazika!</t>
+  </si>
+  <si>
+    <t>ok..</t>
+  </si>
+  <si>
+    <t>LEGO -&gt; Lukasz L, Arduino -&gt; Marcin M., Scratch -&gt; Krzysiu
+Lukasz L -&gt; wgrac!!</t>
+  </si>
+  <si>
+    <t>baterie sa</t>
+  </si>
+  <si>
+    <t>pizzastation -&gt; 12:45!!!
+Jemy na 5.</t>
+  </si>
+  <si>
+    <t>!</t>
   </si>
 </sst>
 </file>
@@ -674,15 +730,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
     <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" customWidth="1"/>
@@ -695,29 +751,29 @@
     <row r="1" spans="1:12">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I1" s="1"/>
       <c r="K1" t="s">
         <v>6</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="64.5" customHeight="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="74.25" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -725,28 +781,28 @@
         <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="96.75" customHeight="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="114" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -754,25 +810,25 @@
         <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>18</v>
+        <v>79</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -786,258 +842,306 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="55.7109375" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.5703125" customWidth="1"/>
+    <col min="4" max="4" width="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="7" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>59</v>
+        <v>51</v>
+      </c>
+      <c r="D3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="60">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>56</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>66</v>
+      </c>
+      <c r="D8" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="8" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>53</v>
+      </c>
+      <c r="D10" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>54</v>
+      </c>
+      <c r="D13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="45">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>55</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>57</v>
+      </c>
+      <c r="D15" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>58</v>
+      </c>
+      <c r="D16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>69</v>
-      </c>
-      <c r="B19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>72</v>
-      </c>
-      <c r="B22" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" t="s">
-        <v>73</v>
+      <c r="D22" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
 </file>
</xml_diff>